<commit_message>
update code and models
</commit_message>
<xml_diff>
--- a/indicators/results.xlsx
+++ b/indicators/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huaichang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huaichang/github/RDEIC/indicators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805996F1-3B1D-684D-96A0-737BC8A72ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE82863-9BFD-F04D-94C9-034A0CB65090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="2140" windowWidth="32000" windowHeight="17500" activeTab="1" xr2:uid="{020B1049-8627-E044-B289-FED9C51C42F8}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="2" xr2:uid="{020B1049-8627-E044-B289-FED9C51C42F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Kodak" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
   <si>
     <t>bpp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,10 +139,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>RDEIC</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SSIM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -168,6 +164,14 @@
   </si>
   <si>
     <t>VQIR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RDEIC-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RDEIC-5</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC44892-1CB9-AF4E-B3F0-6FEAF42E3A70}">
   <dimension ref="A1:P84"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+    <sheetView topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -588,7 +592,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -600,7 +604,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -621,7 +625,7 @@
         <v>19</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1339,7 +1343,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -1557,7 +1561,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -1624,25 +1628,25 @@
         <v>3</v>
       </c>
       <c r="B46" s="1">
-        <v>6.5419514973958301E-2</v>
+        <v>6.5534803602430497E-2</v>
       </c>
       <c r="C46" s="1">
-        <v>0.12189999999999999</v>
+        <v>0.1227</v>
       </c>
       <c r="D46" s="1">
         <v>0.85519999999999996</v>
       </c>
       <c r="E46" s="1">
-        <v>3.3935</v>
+        <v>3.4121000000000001</v>
       </c>
       <c r="F46" s="1">
-        <v>24.49</v>
+        <v>24.5</v>
       </c>
       <c r="G46" s="1">
-        <v>8.9351440469423907E-2</v>
+        <v>8.7940240899721703E-2</v>
       </c>
       <c r="H46" s="1">
-        <v>0.64270000000000005</v>
+        <v>0.64449999999999996</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1650,25 +1654,25 @@
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>4.3626573350694399E-2</v>
+        <v>4.2934841579861098E-2</v>
       </c>
       <c r="C47" s="1">
-        <v>0.15559999999999999</v>
+        <v>0.15959999999999999</v>
       </c>
       <c r="D47" s="1">
-        <v>0.81259999999999999</v>
+        <v>0.81089999999999995</v>
       </c>
       <c r="E47" s="1">
-        <v>3.3559000000000001</v>
+        <v>3.3729</v>
       </c>
       <c r="F47" s="1">
-        <v>23.51</v>
+        <v>23.45</v>
       </c>
       <c r="G47" s="1">
-        <v>0.113217001159985</v>
+        <v>0.118129300574461</v>
       </c>
       <c r="H47" s="1">
-        <v>0.60599999999999998</v>
+        <v>0.60429999999999995</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1676,30 +1680,30 @@
         <v>5</v>
       </c>
       <c r="B48" s="1">
-        <v>2.3769802517361101E-2</v>
+        <v>2.4464925130208301E-2</v>
       </c>
       <c r="C48" s="1">
-        <v>0.2034</v>
+        <v>0.21929999999999999</v>
       </c>
       <c r="D48" s="1">
-        <v>0.75270000000000004</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="E48" s="1">
-        <v>3.3267000000000002</v>
+        <v>3.2624</v>
       </c>
       <c r="F48" s="1">
-        <v>22.21</v>
+        <v>22.37</v>
       </c>
       <c r="G48" s="1">
-        <v>0.14141785353422101</v>
+        <v>0.15459137906630799</v>
       </c>
       <c r="H48" s="1">
-        <v>0.55659999999999998</v>
+        <v>0.55669999999999997</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -1713,39 +1717,169 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>28</v>
+      <c r="B50" s="1">
+        <v>0.12011379665798599</v>
       </c>
       <c r="C50" s="1">
+        <v>8.5599999999999996E-2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E50" s="1">
+        <v>3.5154000000000001</v>
+      </c>
+      <c r="F50" s="1">
+        <v>25.81</v>
+      </c>
+      <c r="G50" s="1">
+        <v>6.2424438695112799E-2</v>
+      </c>
+      <c r="H50" s="1">
+        <v>0.69399999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1">
+        <v>9.0637207031249903E-2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0.1002</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.88329999999999997</v>
+      </c>
+      <c r="E51" s="1">
+        <v>3.4337</v>
+      </c>
+      <c r="F51" s="1">
+        <v>25.31</v>
+      </c>
+      <c r="G51" s="1">
+        <v>7.2540362675984696E-2</v>
+      </c>
+      <c r="H51" s="1">
+        <v>0.67479999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6.5419514973958301E-2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0.12189999999999999</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.85519999999999996</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3.3935</v>
+      </c>
+      <c r="F52" s="1">
+        <v>24.49</v>
+      </c>
+      <c r="G52" s="1">
+        <v>8.9351440469423907E-2</v>
+      </c>
+      <c r="H52" s="1">
+        <v>0.64270000000000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>4.3626573350694399E-2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.15559999999999999</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.81259999999999999</v>
+      </c>
+      <c r="E53" s="1">
+        <v>3.3559000000000001</v>
+      </c>
+      <c r="F53" s="1">
+        <v>23.51</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0.113217001159985</v>
+      </c>
+      <c r="H53" s="1">
+        <v>0.60599999999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2.3769802517361101E-2</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.2034</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.75270000000000004</v>
+      </c>
+      <c r="E54" s="1">
+        <v>3.3267000000000002</v>
+      </c>
+      <c r="F54" s="1">
+        <v>22.21</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0.14141785353422101</v>
+      </c>
+      <c r="H54" s="1">
+        <v>0.55659999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1">
         <v>7.2599999999999998E-2</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D56" s="1">
         <v>0.92490000000000006</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E56" s="1">
         <v>3.4422999999999999</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F56" s="1">
         <v>26.65</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G56" s="1">
         <v>4.14690325657526E-2</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H56" s="1">
         <v>0.72889999999999999</v>
       </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="B51"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="B52"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="B53"/>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="B54"/>
     </row>
     <row r="64" spans="1:10">
       <c r="H64"/>
@@ -1792,13 +1926,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K83:M88">
     <sortCondition ref="K88"/>
   </sortState>
-  <mergeCells count="13">
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A29:H29"/>
-    <mergeCell ref="A26:H26"/>
-    <mergeCell ref="A22:H22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A8:H8"/>
+  <mergeCells count="14">
     <mergeCell ref="A33:H33"/>
     <mergeCell ref="F79:J79"/>
     <mergeCell ref="L79:P79"/>
@@ -1806,6 +1934,13 @@
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A36:H36"/>
     <mergeCell ref="A49:H49"/>
+    <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6E4BF7-ED45-3548-AB34-E0507753F87D}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:J43"/>
+    <sheetView topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1828,7 +1963,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1842,7 +1977,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1869,7 +2004,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -2744,7 +2879,7 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
@@ -3010,7 +3145,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -3091,31 +3226,31 @@
         <v>3</v>
       </c>
       <c r="B46" s="1">
-        <v>6.3462611607142796E-2</v>
+        <v>6.3609095982142802E-2</v>
       </c>
       <c r="C46" s="1">
-        <v>8.4900000000000003E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D46" s="1">
-        <v>0.90869999999999995</v>
+        <v>0.90839999999999999</v>
       </c>
       <c r="E46" s="1">
-        <v>19.317102879922</v>
+        <v>19.197235292551198</v>
       </c>
       <c r="F46" s="1">
-        <v>4.5691593144390102E-4</v>
+        <v>4.30547957925275E-4</v>
       </c>
       <c r="G46" s="1">
-        <v>4.4301000000000004</v>
+        <v>4.4527000000000001</v>
       </c>
       <c r="H46" s="1">
-        <v>25.88</v>
+        <v>25.92</v>
       </c>
       <c r="I46" s="1">
-        <v>7.8137182763644605E-2</v>
+        <v>7.7021931750433703E-2</v>
       </c>
       <c r="J46" s="1">
-        <v>0.7631</v>
+        <v>0.7641</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -3123,31 +3258,31 @@
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>4.23118954613095E-2</v>
+        <v>4.2181299603174599E-2</v>
       </c>
       <c r="C47" s="1">
-        <v>0.1114</v>
+        <v>0.11360000000000001</v>
       </c>
       <c r="D47" s="1">
-        <v>0.87729999999999997</v>
+        <v>0.87590000000000001</v>
       </c>
       <c r="E47" s="1">
-        <v>25.1166174877991</v>
+        <v>25.4276023082884</v>
       </c>
       <c r="F47" s="1">
-        <v>8.5684310555555999E-4</v>
+        <v>9.08393750849256E-4</v>
       </c>
       <c r="G47" s="1">
-        <v>4.4267000000000003</v>
+        <v>4.4569999999999999</v>
       </c>
       <c r="H47" s="1">
-        <v>24.55</v>
+        <v>24.46</v>
       </c>
       <c r="I47" s="1">
-        <v>0.101947490232331</v>
+        <v>0.103385246225765</v>
       </c>
       <c r="J47" s="1">
-        <v>0.72750000000000004</v>
+        <v>0.72609999999999997</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -3155,36 +3290,36 @@
         <v>5</v>
       </c>
       <c r="B48" s="1">
-        <v>2.3876953124999999E-2</v>
+        <v>2.43233816964285E-2</v>
       </c>
       <c r="C48" s="1">
-        <v>0.15629999999999999</v>
+        <v>0.16220000000000001</v>
       </c>
       <c r="D48" s="1">
-        <v>0.82709999999999995</v>
+        <v>0.82379999999999998</v>
       </c>
       <c r="E48" s="1">
-        <v>33.242611347314302</v>
+        <v>34.810863885151797</v>
       </c>
       <c r="F48" s="1">
-        <v>1.55511352126964E-3</v>
+        <v>1.6129266026124499E-3</v>
       </c>
       <c r="G48" s="1">
-        <v>4.5182000000000002</v>
+        <v>4.5419</v>
       </c>
       <c r="H48" s="1">
-        <v>22.59</v>
+        <v>22.81</v>
       </c>
       <c r="I48" s="1">
-        <v>0.13162332006863101</v>
+        <v>0.13996749903474501</v>
       </c>
       <c r="J48" s="1">
-        <v>0.67520000000000002</v>
+        <v>0.67490000000000006</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -3200,36 +3335,211 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>28</v>
+      <c r="B50" s="1">
+        <v>0.118363250248015</v>
       </c>
       <c r="C50" s="1">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="E50" s="1">
+        <v>12.800269795620499</v>
+      </c>
+      <c r="F50" s="5">
+        <v>-1.15982120961977E-4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>4.3243</v>
+      </c>
+      <c r="H50" s="1">
+        <v>27.83</v>
+      </c>
+      <c r="I50" s="1">
+        <v>5.2014158027512601E-2</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.80330000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1">
+        <v>8.8816421750991997E-2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>6.7799999999999999E-2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.9274</v>
+      </c>
+      <c r="E51" s="1">
+        <v>15.2548051208144</v>
+      </c>
+      <c r="F51" s="5">
+        <v>5.8829986561859098E-5</v>
+      </c>
+      <c r="G51" s="1">
+        <v>4.3506</v>
+      </c>
+      <c r="H51" s="1">
+        <v>27.03</v>
+      </c>
+      <c r="I51" s="1">
+        <v>6.1008147682462398E-2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.78790000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>6.3462611607142796E-2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>8.4900000000000003E-2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.90869999999999995</v>
+      </c>
+      <c r="E52" s="1">
+        <v>19.317102879922</v>
+      </c>
+      <c r="F52" s="1">
+        <v>4.5691593144390102E-4</v>
+      </c>
+      <c r="G52" s="1">
+        <v>4.4301000000000004</v>
+      </c>
+      <c r="H52" s="1">
+        <v>25.88</v>
+      </c>
+      <c r="I52" s="1">
+        <v>7.8137182763644605E-2</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.7631</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>4.23118954613095E-2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.1114</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.87729999999999997</v>
+      </c>
+      <c r="E53" s="1">
+        <v>25.1166174877991</v>
+      </c>
+      <c r="F53" s="1">
+        <v>8.5684310555555999E-4</v>
+      </c>
+      <c r="G53" s="1">
+        <v>4.4267000000000003</v>
+      </c>
+      <c r="H53" s="1">
+        <v>24.55</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.101947490232331</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.72750000000000004</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2.3876953124999999E-2</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.82709999999999995</v>
+      </c>
+      <c r="E54" s="1">
+        <v>33.242611347314302</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1.55511352126964E-3</v>
+      </c>
+      <c r="G54" s="1">
+        <v>4.5182000000000002</v>
+      </c>
+      <c r="H54" s="1">
+        <v>22.59</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.13162332006863101</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.67520000000000002</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1">
         <v>4.7699999999999999E-2</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D56" s="1">
         <v>0.95350000000000001</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E56" s="1">
         <v>9.1215484837904306</v>
       </c>
-      <c r="F50" s="1">
+      <c r="F56" s="1">
         <v>-2.5638451269420698E-4</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G56" s="1">
         <v>4.3216999999999999</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H56" s="1">
         <v>29.08</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I56" s="1">
         <v>3.4646058082580498E-2</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J56" s="1">
         <v>0.82850000000000001</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A55:J55"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="A43:J43"/>
@@ -3250,10 +3560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42852A4-F392-0847-A851-0E2120D088FC}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3263,7 +3573,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -3304,7 +3614,7 @@
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -4445,7 +4755,7 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -4526,31 +4836,31 @@
         <v>3</v>
       </c>
       <c r="B46" s="1">
-        <v>5.8326792494158897E-2</v>
+        <v>5.8441510700610003E-2</v>
       </c>
       <c r="C46" s="1">
-        <v>9.9500000000000005E-2</v>
+        <v>9.9400000000000002E-2</v>
       </c>
       <c r="D46" s="1">
         <v>0.89810000000000001</v>
       </c>
       <c r="E46" s="1">
-        <v>8.2677794747640405</v>
+        <v>7.9722310313514404</v>
       </c>
       <c r="F46" s="1">
-        <v>6.4819457078146804E-4</v>
+        <v>4.5730658880707101E-4</v>
       </c>
       <c r="G46" s="1">
-        <v>3.8496999999999999</v>
+        <v>3.8147000000000002</v>
       </c>
       <c r="H46" s="1">
-        <v>25.99</v>
+        <v>26.05</v>
       </c>
       <c r="I46" s="1">
-        <v>8.0424914571726402E-2</v>
+        <v>7.9080154266312805E-2</v>
       </c>
       <c r="J46" s="1">
-        <v>0.74960000000000004</v>
+        <v>0.75029999999999997</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -4558,31 +4868,31 @@
         <v>4</v>
       </c>
       <c r="B47" s="1">
-        <v>3.8242993696456298E-2</v>
+        <v>3.7863853193146398E-2</v>
       </c>
       <c r="C47" s="1">
-        <v>0.13170000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D47" s="1">
-        <v>0.86319999999999997</v>
+        <v>0.86140000000000005</v>
       </c>
       <c r="E47" s="1">
-        <v>11.443965436804</v>
+        <v>11.4751650695652</v>
       </c>
       <c r="F47" s="1">
-        <v>1.09171910251761E-3</v>
+        <v>1.1811205068235501E-3</v>
       </c>
       <c r="G47" s="1">
-        <v>3.8567</v>
+        <v>3.8285999999999998</v>
       </c>
       <c r="H47" s="1">
-        <v>24.75</v>
+        <v>24.69</v>
       </c>
       <c r="I47" s="1">
-        <v>0.10562073293133301</v>
+        <v>0.108475327213233</v>
       </c>
       <c r="J47" s="1">
-        <v>0.71550000000000002</v>
+        <v>0.71330000000000005</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -4590,36 +4900,36 @@
         <v>5</v>
       </c>
       <c r="B48" s="1">
-        <v>2.0905079747533702E-2</v>
+        <v>2.11496006538811E-2</v>
       </c>
       <c r="C48" s="1">
-        <v>0.17749999999999999</v>
+        <v>0.18990000000000001</v>
       </c>
       <c r="D48" s="1">
-        <v>0.81189999999999996</v>
+        <v>0.80669999999999997</v>
       </c>
       <c r="E48" s="1">
-        <v>15.3349770421123</v>
+        <v>16.928723093032101</v>
       </c>
       <c r="F48" s="1">
-        <v>1.5915192148181899E-3</v>
+        <v>2.1572153946213001E-3</v>
       </c>
       <c r="G48" s="1">
-        <v>3.9588999999999999</v>
+        <v>3.9870000000000001</v>
       </c>
       <c r="H48" s="1">
-        <v>23.03</v>
+        <v>23.28</v>
       </c>
       <c r="I48" s="1">
-        <v>0.13413119246469399</v>
+        <v>0.14551580021871499</v>
       </c>
       <c r="J48" s="1">
-        <v>0.66839999999999999</v>
+        <v>0.66679999999999995</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
@@ -4635,42 +4945,211 @@
       <c r="A50" s="1">
         <v>1</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>28</v>
+      <c r="B50" s="1">
+        <v>0.11082805502823199</v>
       </c>
       <c r="C50" s="1">
+        <v>6.6600000000000006E-2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="E50" s="1">
+        <v>5.2404533504275097</v>
+      </c>
+      <c r="F50" s="5">
+        <v>1.7950364576613199E-4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>3.7793000000000001</v>
+      </c>
+      <c r="H50" s="1">
+        <v>27.8</v>
+      </c>
+      <c r="I50" s="1">
+        <v>5.3594543415809298E-2</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0.7903</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>2</v>
+      </c>
+      <c r="B51" s="1">
+        <v>8.2307461018626599E-2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.92</v>
+      </c>
+      <c r="E51" s="1">
+        <v>6.3040800568844499</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2.44471199078066E-4</v>
+      </c>
+      <c r="G51" s="1">
+        <v>3.7875000000000001</v>
+      </c>
+      <c r="H51" s="1">
+        <v>27.08</v>
+      </c>
+      <c r="I51" s="1">
+        <v>6.2894869212792304E-2</v>
+      </c>
+      <c r="J51" s="1">
+        <v>0.77470000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>5.8326792494158897E-2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>9.9500000000000005E-2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="E52" s="1">
+        <v>8.2677794747640405</v>
+      </c>
+      <c r="F52" s="1">
+        <v>6.4819457078146804E-4</v>
+      </c>
+      <c r="G52" s="1">
+        <v>3.8496999999999999</v>
+      </c>
+      <c r="H52" s="1">
+        <v>25.99</v>
+      </c>
+      <c r="I52" s="1">
+        <v>8.0424914571726402E-2</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0.74960000000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
+        <v>3.8242993696456298E-2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0.13170000000000001</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.86319999999999997</v>
+      </c>
+      <c r="E53" s="1">
+        <v>11.443965436804</v>
+      </c>
+      <c r="F53" s="1">
+        <v>1.09171910251761E-3</v>
+      </c>
+      <c r="G53" s="1">
+        <v>3.8567</v>
+      </c>
+      <c r="H53" s="1">
+        <v>24.75</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0.10562073293133301</v>
+      </c>
+      <c r="J53" s="1">
+        <v>0.71550000000000002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>5</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2.0905079747533702E-2</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0.17749999999999999</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.81189999999999996</v>
+      </c>
+      <c r="E54" s="1">
+        <v>15.3349770421123</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1.5915192148181899E-3</v>
+      </c>
+      <c r="G54" s="1">
+        <v>3.9588999999999999</v>
+      </c>
+      <c r="H54" s="1">
+        <v>23.03</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0.13413119246469399</v>
+      </c>
+      <c r="J54" s="1">
+        <v>0.66839999999999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>1</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="1">
         <v>5.45E-2</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D56" s="1">
         <v>0.95040000000000002</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E56" s="1">
         <v>3.5671577634753899</v>
       </c>
-      <c r="F50" s="5">
+      <c r="F56" s="5">
         <v>-4.6106953788349599E-5</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G56" s="1">
         <v>3.8549000000000002</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H56" s="1">
         <v>28.85</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I56" s="1">
         <v>3.4095323252900697E-2</v>
       </c>
-      <c r="J50" s="1">
+      <c r="J56" s="1">
         <v>0.81589999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
-      <c r="F51" s="5"/>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="F52" s="5"/>
-    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A55:J55"/>
     <mergeCell ref="A49:J49"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A15:J15"/>

</xml_diff>